<commit_message>
add measurements at 200MHz for Baremetal CPU and DMA simultaneusly
</commit_message>
<xml_diff>
--- a/results/CPU and DMA simultaneously.xlsx
+++ b/results/CPU and DMA simultaneously.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roberto.fernandez\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roberto.fernandez\git\Zynq7000-time-measurements\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9462C07-2313-45E1-A65A-7A01FE60FE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FFC8E23-5521-4505-9503-FE247231173F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{97C2288C-4D36-48FC-BB8D-9391E86D55EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Baremetal, FPGA Frequency 150MHz</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>CPU</t>
   </si>
@@ -55,12 +53,27 @@
   <si>
     <t>CPU+DMA</t>
   </si>
+  <si>
+    <t>FPGA frequency = 150MHz</t>
+  </si>
+  <si>
+    <t>FPGA frequency = 200MHz</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed </t>
+  </si>
+  <si>
+    <t>Baremetal / CPU GP1 DMA GP0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,13 +81,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aharoni"/>
+      <charset val="177"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -206,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -221,6 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -239,12 +277,26 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD10909"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -270,6 +322,61 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>150MHz</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
@@ -1206,7 +1313,1023 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>200MHz</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.1925952618854237E-2"/>
+          <c:y val="3.6742920281013641E-2"/>
+          <c:w val="0.88031360783958967"/>
+          <c:h val="0.82065415231310079"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CPU WR</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$F$4:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>37.398992800245097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.119594029017861</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>149.59597120098039</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>282.57016782407408</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>469.50120192307691</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>701.55352011494256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>878.2036870503598</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>529.58920824295012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>440.68704873646209</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>411.87789962041336</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>395.04955501618127</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>388.37243984887652</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>384.94703128849466</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>382.95630009068407</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>382.2115678624283</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>381.83795408169499</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>381.62112654556552</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>381.54774077951731</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>381.50174346296762</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>381.06735441702796</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>380.98924619753683</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4AE3-4F63-A1E4-AF694131196C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>DMA WR</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$G$4:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.0199725309157754</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0421291571868307</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0388536428004231</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2036500336021501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.095769053270043</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.236006269191403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58.885823685479984</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104.78138412017167</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>172.23324514991182</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>253.98244473342004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>333.69639501110544</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>394.8898099474323</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>434.38976925215457</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>457.68768856732771</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>469.83296498428876</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>470.07679174469939</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>470.1227584546877</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>470.17138687394333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>470.06795302328908</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>470.03768292103973</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>470.0482880606325</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4AE3-4F63-A1E4-AF694131196C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>DMA + CPU WR</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$H$4:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.0543662978510226</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0619985219594597</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1329331155200437</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8694115845796802</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.04499375657203</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.575352431453698</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63.479101664066562</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>118.91896005845105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>211.65203727785001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>347.16050479914679</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>497.10486128785948</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>625.80102531239982</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>691.86149486362024</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>724.82256343647077</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>743.33967649857277</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>750.67861346657378</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>750.71468037571765</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>751.16580933608964</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>751.30012486608075</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>750.69777358054307</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>749.20425143444515</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4AE3-4F63-A1E4-AF694131196C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>CPU RD</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$F$25:$F$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>34.059797014508931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.86406525088028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>136.23918805803572</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.38677014802632</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>113.44824581784387</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>156.90271529562983</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>167.44898834019205</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>173.88933404558404</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>176.72140788997467</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>238.30222059541236</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>242.98643941278925</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>245.52168447517286</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>250.68185464463343</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>253.04873111244268</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>253.12046914360232</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>253.08664471899286</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>253.08818199672402</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>253.08895064259283</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>251.35480238485437</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>246.1410619657662</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>245.99553099918836</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4AE3-4F63-A1E4-AF694131196C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>DMA RD</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$G$25:$G$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.0167103586420576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0619985219594592</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0345819837387626</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2036500336021501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.155414571201693</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.284037032291131</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58.715879028379028</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104.87140249140893</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>172.53754416961129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>254.37939567595728</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>326.4457629951529</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>373.44646271510516</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>402.18790218790218</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>418.46326896810302</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>426.48724632538585</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>426.734762155113</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>426.81344496496718</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>426.8389502493593</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>426.79595738869165</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>426.74714548834379</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>426.76116865985472</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4AE3-4F63-A1E4-AF694131196C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>CPU+DMA RD</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$H$25:$H$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.0685426514355743</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1040801244484282</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1896729990389892</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.9680360639686683</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.22412446836789</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.905465891270257</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.078904199475062</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120.20710241260463</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>189.25629844961242</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256.78740468051541</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>385.53592577970784</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>451.95533958116397</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>493.36911904010105</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>525.42201896563324</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>542.50646667708281</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>547.97643262958547</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>542.10649573687454</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>541.13022623572499</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>538.53718222267219</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>535.47294041042926</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>534.53682517732591</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4AE3-4F63-A1E4-AF694131196C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="474689768"/>
+        <c:axId val="474691408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="474689768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>n (data size </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>2n</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474691408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="474691408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Transfer rate (MB/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474689768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.661612668907436E-2"/>
+          <c:y val="4.9240427972411197E-2"/>
+          <c:w val="0.24077339704714998"/>
+          <c:h val="0.32203105963538142"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1762,20 +2885,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>148973</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>63933</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>146412</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63934</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>648035</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>13109</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>651237</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>13110</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1795,6 +3434,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>149837</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>162005</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>631370</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8782154-4665-42BD-92C7-06B31F722972}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2100,10 +3777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18302C3F-120B-4B05-BB40-807F2AA77811}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2111,33 +3788,59 @@
     <col min="1" max="1" width="6.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+      <c r="D3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>37.398992800245097</v>
       </c>
       <c r="D4" s="3">
@@ -2146,13 +3849,22 @@
       <c r="E4" s="4">
         <v>1.0514601062913451</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+      <c r="F4" s="2">
+        <v>37.398992800245097</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.0199725309157754</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.0543662978510226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
       <c r="B5" s="5">
         <v>4</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>68.119594029017861</v>
       </c>
       <c r="D5" s="6">
@@ -2161,15 +3873,22 @@
       <c r="E5" s="7">
         <v>2.0586601541419318</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
+      <c r="F5" s="5">
+        <v>68.119594029017861</v>
+      </c>
+      <c r="G5" s="6">
+        <v>2.0421291571868307</v>
+      </c>
+      <c r="H5" s="7">
+        <v>2.0619985219594597</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
       <c r="B6" s="5">
         <v>8</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>149.59597120098039</v>
       </c>
       <c r="D6" s="6">
@@ -2178,15 +3897,22 @@
       <c r="E6" s="7">
         <v>4.1351731876693769</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="F6" s="5">
+        <v>149.59597120098039</v>
+      </c>
+      <c r="G6" s="6">
+        <v>4.0388536428004231</v>
+      </c>
+      <c r="H6" s="7">
+        <v>4.1329331155200437</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
       <c r="B7" s="5">
         <v>16</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>282.57016782407408</v>
       </c>
       <c r="D7" s="6">
@@ -2195,15 +3921,22 @@
       <c r="E7" s="7">
         <v>7.8816059207128104</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
+      <c r="F7" s="5">
+        <v>282.57016782407408</v>
+      </c>
+      <c r="G7" s="6">
+        <v>8.2036500336021501</v>
+      </c>
+      <c r="H7" s="7">
+        <v>7.8694115845796802</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
       <c r="B8" s="5">
         <v>32</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>469.50120192307691</v>
       </c>
       <c r="D8" s="6">
@@ -2212,15 +3945,22 @@
       <c r="E8" s="7">
         <v>16.070341298051606</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
+      <c r="F8" s="5">
+        <v>469.50120192307691</v>
+      </c>
+      <c r="G8" s="6">
+        <v>16.095769053270043</v>
+      </c>
+      <c r="H8" s="7">
+        <v>16.04499375657203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
       <c r="B9" s="5">
         <v>64</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>709.71111918604652</v>
       </c>
       <c r="D9" s="6">
@@ -2229,15 +3969,22 @@
       <c r="E9" s="7">
         <v>31.575352431453698</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
+      <c r="F9" s="5">
+        <v>701.55352011494256</v>
+      </c>
+      <c r="G9" s="6">
+        <v>31.236006269191403</v>
+      </c>
+      <c r="H9" s="7">
+        <v>31.575352431453698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
       <c r="B10" s="5">
         <v>128</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>865.74689716312048</v>
       </c>
       <c r="D10" s="6">
@@ -2246,15 +3993,22 @@
       <c r="E10" s="7">
         <v>63.479101664066569</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
+      <c r="F10" s="5">
+        <v>878.2036870503598</v>
+      </c>
+      <c r="G10" s="6">
+        <v>58.885823685479984</v>
+      </c>
+      <c r="H10" s="7">
+        <v>63.479101664066562</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
       <c r="B11" s="5">
         <v>256</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>408.26191471571906</v>
       </c>
       <c r="D11" s="6">
@@ -2263,15 +4017,22 @@
       <c r="E11" s="7">
         <v>118.74544017509727</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
+      <c r="F11" s="5">
+        <v>529.58920824295012</v>
+      </c>
+      <c r="G11" s="6">
+        <v>104.78138412017167</v>
+      </c>
+      <c r="H11" s="7">
+        <v>118.91896005845105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
       <c r="B12" s="5">
         <v>512</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>325.95544058744991</v>
       </c>
       <c r="D12" s="6">
@@ -2280,15 +4041,22 @@
       <c r="E12" s="7">
         <v>211.01177614520313</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
+      <c r="F12" s="5">
+        <v>440.68704873646209</v>
+      </c>
+      <c r="G12" s="6">
+        <v>172.23324514991182</v>
+      </c>
+      <c r="H12" s="7">
+        <v>211.65203727785001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
       <c r="B13" s="5">
         <v>1024</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>297.91412446613788</v>
       </c>
       <c r="D13" s="6">
@@ -2297,15 +4065,22 @@
       <c r="E13" s="7">
         <v>312.60003201024324</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
+      <c r="F13" s="5">
+        <v>411.87789962041336</v>
+      </c>
+      <c r="G13" s="6">
+        <v>253.98244473342004</v>
+      </c>
+      <c r="H13" s="7">
+        <v>347.16050479914679</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
       <c r="B14" s="5">
         <v>2048</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>284.09090909090907</v>
       </c>
       <c r="D14" s="6">
@@ -2314,15 +4089,22 @@
       <c r="E14" s="7">
         <v>407.41030454735085</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
+      <c r="F14" s="5">
+        <v>395.04955501618127</v>
+      </c>
+      <c r="G14" s="6">
+        <v>333.69639501110544</v>
+      </c>
+      <c r="H14" s="7">
+        <v>497.10486128785948</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
       <c r="B15" s="5">
         <v>4096</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>278.28239652347366</v>
       </c>
       <c r="D15" s="6">
@@ -2331,15 +4113,22 @@
       <c r="E15" s="7">
         <v>486.57822620827102</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
+      <c r="F15" s="5">
+        <v>388.37243984887652</v>
+      </c>
+      <c r="G15" s="6">
+        <v>394.8898099474323</v>
+      </c>
+      <c r="H15" s="7">
+        <v>625.80102531239982</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="19"/>
       <c r="B16" s="5">
         <v>8192</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>275.38862843244385</v>
       </c>
       <c r="D16" s="6">
@@ -2348,15 +4137,22 @@
       <c r="E16" s="7">
         <v>514.1155567254541</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
+      <c r="F16" s="5">
+        <v>384.94703128849466</v>
+      </c>
+      <c r="G16" s="6">
+        <v>434.38976925215457</v>
+      </c>
+      <c r="H16" s="7">
+        <v>691.86149486362024</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="19"/>
       <c r="B17" s="5">
         <v>16384</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>273.83935925971366</v>
       </c>
       <c r="D17" s="6">
@@ -2365,15 +4161,22 @@
       <c r="E17" s="7">
         <v>528.67535104043304</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
+      <c r="F17" s="5">
+        <v>382.95630009068407</v>
+      </c>
+      <c r="G17" s="6">
+        <v>457.68768856732771</v>
+      </c>
+      <c r="H17" s="7">
+        <v>724.82256343647077</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="19"/>
       <c r="B18" s="5">
         <v>32768</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>273.12613620472661</v>
       </c>
       <c r="D18" s="6">
@@ -2382,15 +4185,22 @@
       <c r="E18" s="7">
         <v>536.56358922408606</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
+      <c r="F18" s="5">
+        <v>382.2115678624283</v>
+      </c>
+      <c r="G18" s="6">
+        <v>469.83296498428876</v>
+      </c>
+      <c r="H18" s="7">
+        <v>743.33967649857277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="19"/>
       <c r="B19" s="5">
         <v>65536</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>272.81377949662584</v>
       </c>
       <c r="D19" s="6">
@@ -2399,15 +4209,22 @@
       <c r="E19" s="7">
         <v>539.62114278807132</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
+      <c r="F19" s="5">
+        <v>381.83795408169499</v>
+      </c>
+      <c r="G19" s="6">
+        <v>470.07679174469939</v>
+      </c>
+      <c r="H19" s="7">
+        <v>750.67861346657378</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="19"/>
       <c r="B20" s="5">
         <v>131072</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>272.62813522355509</v>
       </c>
       <c r="D20" s="6">
@@ -2416,15 +4233,22 @@
       <c r="E20" s="7">
         <v>539.69569797765223</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
+      <c r="F20" s="5">
+        <v>381.62112654556552</v>
+      </c>
+      <c r="G20" s="6">
+        <v>470.1227584546877</v>
+      </c>
+      <c r="H20" s="7">
+        <v>750.71468037571765</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="19"/>
       <c r="B21" s="5">
         <v>262144</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>272.5550179559246</v>
       </c>
       <c r="D21" s="6">
@@ -2433,15 +4257,22 @@
       <c r="E21" s="7">
         <v>539.94864008535501</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
+      <c r="F21" s="5">
+        <v>381.54774077951731</v>
+      </c>
+      <c r="G21" s="6">
+        <v>470.17138687394333</v>
+      </c>
+      <c r="H21" s="7">
+        <v>751.16580933608964</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="19"/>
       <c r="B22" s="5">
         <v>524288</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>272.51357253848028</v>
       </c>
       <c r="D22" s="6">
@@ -2450,15 +4281,22 @@
       <c r="E22" s="7">
         <v>540.08103375830513</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
+      <c r="F22" s="5">
+        <v>381.50174346296762</v>
+      </c>
+      <c r="G22" s="6">
+        <v>470.06795302328908</v>
+      </c>
+      <c r="H22" s="7">
+        <v>751.30012486608075</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="19"/>
       <c r="B23" s="5">
         <v>1048576</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>272.44586092074712</v>
       </c>
       <c r="D23" s="6">
@@ -2467,15 +4305,22 @@
       <c r="E23" s="7">
         <v>539.81601990409627</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
+      <c r="F23" s="5">
+        <v>381.06735441702796</v>
+      </c>
+      <c r="G23" s="6">
+        <v>470.03768292103973</v>
+      </c>
+      <c r="H23" s="7">
+        <v>750.69777358054307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="20"/>
       <c r="B24" s="8">
         <v>2097152</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <v>272.44203829690491</v>
       </c>
       <c r="D24" s="9">
@@ -2484,17 +4329,24 @@
       <c r="E24" s="10">
         <v>539.24823942190426</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
-        <v>4</v>
+      <c r="F24" s="8">
+        <v>380.98924619753683</v>
+      </c>
+      <c r="G24" s="9">
+        <v>470.0482880606325</v>
+      </c>
+      <c r="H24" s="10">
+        <v>749.20425143444515</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>3</v>
       </c>
       <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>34.059797014508931</v>
       </c>
       <c r="D25" s="3">
@@ -2503,15 +4355,23 @@
       <c r="E25" s="4">
         <v>1.0661535119130801</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
+      <c r="F25" s="2">
+        <v>34.059797014508931</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1.0167103586420576</v>
+      </c>
+      <c r="H25" s="4">
+        <v>1.0685426514355743</v>
+      </c>
+      <c r="P25" s="14"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
       <c r="B26" s="5">
         <v>4</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>23.403050709355831</v>
       </c>
       <c r="D26" s="6">
@@ -2520,15 +4380,22 @@
       <c r="E26" s="7">
         <v>2.1006042211591414</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
+      <c r="F26" s="5">
+        <v>26.86406525088028</v>
+      </c>
+      <c r="G26" s="6">
+        <v>2.0619985219594592</v>
+      </c>
+      <c r="H26" s="7">
+        <v>2.1040801244484282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
       <c r="B27" s="5">
         <v>8</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>136.23918805803572</v>
       </c>
       <c r="D27" s="6">
@@ -2537,15 +4404,22 @@
       <c r="E27" s="7">
         <v>4.1965866508525851</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
+      <c r="F27" s="5">
+        <v>136.23918805803572</v>
+      </c>
+      <c r="G27" s="6">
+        <v>4.0345819837387626</v>
+      </c>
+      <c r="H27" s="7">
+        <v>4.1896729990389892</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="16"/>
       <c r="B28" s="5">
         <v>16</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>87.193080357142861</v>
       </c>
       <c r="D28" s="6">
@@ -2554,15 +4428,22 @@
       <c r="E28" s="7">
         <v>7.9348877080083211</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
+      <c r="F28" s="5">
+        <v>100.38677014802632</v>
+      </c>
+      <c r="G28" s="6">
+        <v>8.2036500336021501</v>
+      </c>
+      <c r="H28" s="7">
+        <v>7.9680360639686683</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="16"/>
       <c r="B29" s="5">
         <v>32</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>97.189739251592357</v>
       </c>
       <c r="D29" s="6">
@@ -2571,15 +4452,22 @@
       <c r="E29" s="7">
         <v>16.198289875265392</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
+      <c r="F29" s="5">
+        <v>113.44824581784387</v>
+      </c>
+      <c r="G29" s="6">
+        <v>16.155414571201693</v>
+      </c>
+      <c r="H29" s="7">
+        <v>16.22412446836789</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="16"/>
       <c r="B30" s="5">
         <v>64</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>132.39730206073753</v>
       </c>
       <c r="D30" s="6">
@@ -2588,15 +4476,22 @@
       <c r="E30" s="7">
         <v>31.872144255874673</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
+      <c r="F30" s="5">
+        <v>156.90271529562983</v>
+      </c>
+      <c r="G30" s="6">
+        <v>31.284037032291131</v>
+      </c>
+      <c r="H30" s="7">
+        <v>31.905465891270257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
       <c r="B31" s="5">
         <v>128</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>140.31070402298849</v>
       </c>
       <c r="D31" s="6">
@@ -2605,15 +4500,22 @@
       <c r="E31" s="7">
         <v>63.978151205450736</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
+      <c r="F31" s="5">
+        <v>167.44898834019205</v>
+      </c>
+      <c r="G31" s="6">
+        <v>58.715879028379028</v>
+      </c>
+      <c r="H31" s="7">
+        <v>64.078904199475062</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="16"/>
       <c r="B32" s="5">
         <v>256</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>145.3218005952381</v>
       </c>
       <c r="D32" s="6">
@@ -2622,15 +4524,22 @@
       <c r="E32" s="7">
         <v>117.54483630235917</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
+      <c r="F32" s="5">
+        <v>173.88933404558404</v>
+      </c>
+      <c r="G32" s="6">
+        <v>104.87140249140893</v>
+      </c>
+      <c r="H32" s="7">
+        <v>120.20710241260463</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="16"/>
       <c r="B33" s="5">
         <v>512</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>146.76322512774271</v>
       </c>
       <c r="D33" s="6">
@@ -2639,15 +4548,22 @@
       <c r="E33" s="7">
         <v>173.95128250801568</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="15"/>
+      <c r="F33" s="5">
+        <v>176.72140788997467</v>
+      </c>
+      <c r="G33" s="6">
+        <v>172.53754416961129</v>
+      </c>
+      <c r="H33" s="7">
+        <v>189.25629844961242</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
       <c r="B34" s="5">
         <v>1024</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="5">
         <v>198.24654892407634</v>
       </c>
       <c r="D34" s="6">
@@ -2656,15 +4572,22 @@
       <c r="E34" s="7">
         <v>227.37194412107101</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
+      <c r="F34" s="5">
+        <v>238.30222059541236</v>
+      </c>
+      <c r="G34" s="6">
+        <v>254.37939567595728</v>
+      </c>
+      <c r="H34" s="7">
+        <v>256.78740468051541</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
       <c r="B35" s="5">
         <v>2048</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="5">
         <v>202.08225556130367</v>
       </c>
       <c r="D35" s="6">
@@ -2673,15 +4596,22 @@
       <c r="E35" s="7">
         <v>322.67057657359987</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
+      <c r="F35" s="5">
+        <v>242.98643941278925</v>
+      </c>
+      <c r="G35" s="6">
+        <v>326.4457629951529</v>
+      </c>
+      <c r="H35" s="7">
+        <v>385.53592577970784</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="16"/>
       <c r="B36" s="5">
         <v>4096</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="5">
         <v>204.40868655154367</v>
       </c>
       <c r="D36" s="6">
@@ -2690,15 +4620,22 @@
       <c r="E36" s="7">
         <v>368.37514145605434</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
+      <c r="F36" s="5">
+        <v>245.52168447517286</v>
+      </c>
+      <c r="G36" s="6">
+        <v>373.44646271510516</v>
+      </c>
+      <c r="H36" s="7">
+        <v>451.95533958116397</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="16"/>
       <c r="B37" s="5">
         <v>8192</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="5">
         <v>208.8289540509476</v>
       </c>
       <c r="D37" s="6">
@@ -2707,15 +4644,22 @@
       <c r="E37" s="7">
         <v>395.34942563635445</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
+      <c r="F37" s="5">
+        <v>250.68185464463343</v>
+      </c>
+      <c r="G37" s="6">
+        <v>402.18790218790218</v>
+      </c>
+      <c r="H37" s="7">
+        <v>493.36911904010105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="16"/>
       <c r="B38" s="5">
         <v>16384</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="5">
         <v>210.48306705822131</v>
       </c>
       <c r="D38" s="6">
@@ -2724,15 +4668,22 @@
       <c r="E38" s="7">
         <v>415.66906092045758</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
+      <c r="F38" s="5">
+        <v>253.04873111244268</v>
+      </c>
+      <c r="G38" s="6">
+        <v>418.46326896810302</v>
+      </c>
+      <c r="H38" s="7">
+        <v>525.42201896563324</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="16"/>
       <c r="B39" s="5">
         <v>32768</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="5">
         <v>210.42212361373907</v>
       </c>
       <c r="D39" s="6">
@@ -2741,15 +4692,22 @@
       <c r="E39" s="7">
         <v>426.28944029901646</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
+      <c r="F39" s="5">
+        <v>253.12046914360232</v>
+      </c>
+      <c r="G39" s="6">
+        <v>426.48724632538585</v>
+      </c>
+      <c r="H39" s="7">
+        <v>542.50646667708281</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="16"/>
       <c r="B40" s="5">
         <v>65536</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="5">
         <v>210.3817503088404</v>
       </c>
       <c r="D40" s="6">
@@ -2758,15 +4716,22 @@
       <c r="E40" s="7">
         <v>430.49413839181165</v>
       </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
+      <c r="F40" s="5">
+        <v>253.08664471899286</v>
+      </c>
+      <c r="G40" s="6">
+        <v>426.734762155113</v>
+      </c>
+      <c r="H40" s="7">
+        <v>547.97643262958547</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="16"/>
       <c r="B41" s="5">
         <v>131072</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="5">
         <v>210.37891767620496</v>
       </c>
       <c r="D41" s="6">
@@ -2775,15 +4740,22 @@
       <c r="E41" s="7">
         <v>430.52824093049207</v>
       </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="15"/>
+      <c r="F41" s="5">
+        <v>253.08818199672402</v>
+      </c>
+      <c r="G41" s="6">
+        <v>426.81344496496718</v>
+      </c>
+      <c r="H41" s="7">
+        <v>542.10649573687454</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="16"/>
       <c r="B42" s="5">
         <v>262144</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="5">
         <v>210.38228143595163</v>
       </c>
       <c r="D42" s="6">
@@ -2792,15 +4764,22 @@
       <c r="E42" s="7">
         <v>430.60981239191693</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="15"/>
+      <c r="F42" s="5">
+        <v>253.08895064259283</v>
+      </c>
+      <c r="G42" s="6">
+        <v>426.8389502493593</v>
+      </c>
+      <c r="H42" s="7">
+        <v>541.13022623572499</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="16"/>
       <c r="B43" s="5">
         <v>524288</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="5">
         <v>209.7716677351037</v>
       </c>
       <c r="D43" s="6">
@@ -2809,15 +4788,22 @@
       <c r="E43" s="7">
         <v>430.64541689921521</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
+      <c r="F43" s="5">
+        <v>251.35480238485437</v>
+      </c>
+      <c r="G43" s="6">
+        <v>426.79595738869165</v>
+      </c>
+      <c r="H43" s="7">
+        <v>538.53718222267219</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="16"/>
       <c r="B44" s="5">
         <v>1048576</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="5">
         <v>206.56022893483294</v>
       </c>
       <c r="D44" s="6">
@@ -2826,15 +4812,22 @@
       <c r="E44" s="7">
         <v>430.82389900798489</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="16"/>
+      <c r="F44" s="5">
+        <v>246.1410619657662</v>
+      </c>
+      <c r="G44" s="6">
+        <v>426.74714548834379</v>
+      </c>
+      <c r="H44" s="7">
+        <v>535.47294041042926</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="17"/>
       <c r="B45" s="8">
         <v>2097152</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="8">
         <v>206.46050002874961</v>
       </c>
       <c r="D45" s="9">
@@ -2843,15 +4836,574 @@
       <c r="E45" s="10">
         <v>430.88794371224617</v>
       </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
+      <c r="F45" s="8">
+        <v>245.99553099918836</v>
+      </c>
+      <c r="G45" s="9">
+        <v>426.76116865985472</v>
+      </c>
+      <c r="H45" s="10">
+        <v>534.53682517732591</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A25:A45"/>
     <mergeCell ref="A4:A24"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EAB6902-A403-4559-B82F-7233D9E6DD52}">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1809</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1785</v>
+      </c>
+      <c r="D2">
+        <f>$A2*1000000000/(1024*1024*B2)</f>
+        <v>1.0543662978510226</v>
+      </c>
+      <c r="E2" s="1">
+        <f>$A2*1000000000/(1024*1024*C2)</f>
+        <v>1.0685426514355743</v>
+      </c>
+      <c r="I2">
+        <v>1809</v>
+      </c>
+      <c r="J2">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1850</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1813</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:E22" si="0">$A3*1000000000/(1024*1024*B3)</f>
+        <v>2.0619985219594597</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1040801244484282</v>
+      </c>
+      <c r="I3">
+        <v>1850</v>
+      </c>
+      <c r="J3">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1846</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1821</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1329331155200437</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1896729990389892</v>
+      </c>
+      <c r="I4">
+        <v>1846</v>
+      </c>
+      <c r="J4">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1939</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1915</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>7.8694115845796802</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>7.9680360639686683</v>
+      </c>
+      <c r="I5">
+        <v>1939</v>
+      </c>
+      <c r="J5">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1902</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1881</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>16.04499375657203</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>16.22412446836789</v>
+      </c>
+      <c r="I6">
+        <v>1902</v>
+      </c>
+      <c r="J6">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>64</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1933</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1913</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>31.575352431453698</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>31.905465891270257</v>
+      </c>
+      <c r="I7">
+        <v>1933</v>
+      </c>
+      <c r="J7">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>128</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1923</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1905</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>63.479101664066562</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>64.078904199475062</v>
+      </c>
+      <c r="I8">
+        <v>1923</v>
+      </c>
+      <c r="J8">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>256</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2053</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2031</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>118.91896005845105</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>120.20710241260463</v>
+      </c>
+      <c r="I9">
+        <v>2053</v>
+      </c>
+      <c r="J9">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>512</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2307</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2580</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>211.65203727785001</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>189.25629844961242</v>
+      </c>
+      <c r="I10">
+        <v>2307</v>
+      </c>
+      <c r="J10">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1024</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2813</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3803</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>347.16050479914679</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>256.78740468051541</v>
+      </c>
+      <c r="I11">
+        <v>2813</v>
+      </c>
+      <c r="J11">
+        <v>3803</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2048</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3929</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5066</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>497.10486128785948</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>385.53592577970784</v>
+      </c>
+      <c r="I12">
+        <v>3929</v>
+      </c>
+      <c r="J12">
+        <v>5066</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4096</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6242</v>
+      </c>
+      <c r="C13" s="1">
+        <v>8643</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>625.80102531239982</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>451.95533958116397</v>
+      </c>
+      <c r="I13">
+        <v>6242</v>
+      </c>
+      <c r="J13">
+        <v>8643</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>8192</v>
+      </c>
+      <c r="B14" s="1">
+        <v>11292</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15835</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>691.86149486362024</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>493.36911904010105</v>
+      </c>
+      <c r="I14">
+        <v>11292</v>
+      </c>
+      <c r="J14">
+        <v>15835</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>16384</v>
+      </c>
+      <c r="B15" s="1">
+        <v>21557</v>
+      </c>
+      <c r="C15" s="1">
+        <v>29738</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>724.82256343647077</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>525.42201896563324</v>
+      </c>
+      <c r="I15">
+        <v>21557</v>
+      </c>
+      <c r="J15">
+        <v>29738</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>32768</v>
+      </c>
+      <c r="B16" s="1">
+        <v>42040</v>
+      </c>
+      <c r="C16" s="1">
+        <v>57603</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>743.33967649857277</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>542.50646667708281</v>
+      </c>
+      <c r="I16">
+        <v>42040</v>
+      </c>
+      <c r="J16">
+        <v>57603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>65536</v>
+      </c>
+      <c r="B17" s="1">
+        <v>83258</v>
+      </c>
+      <c r="C17" s="1">
+        <v>114056</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>750.67861346657378</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>547.97643262958547</v>
+      </c>
+      <c r="I17">
+        <v>83258</v>
+      </c>
+      <c r="J17">
+        <v>114056</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>131072</v>
+      </c>
+      <c r="B18" s="1">
+        <v>166508</v>
+      </c>
+      <c r="C18" s="1">
+        <v>230582</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>750.71468037571765</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>542.10649573687454</v>
+      </c>
+      <c r="I18">
+        <v>166508</v>
+      </c>
+      <c r="J18">
+        <v>230582</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>262144</v>
+      </c>
+      <c r="B19" s="1">
+        <v>332816</v>
+      </c>
+      <c r="C19" s="1">
+        <v>461996</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>751.16580933608964</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>541.13022623572499</v>
+      </c>
+      <c r="I19">
+        <v>332816</v>
+      </c>
+      <c r="J19">
+        <v>461996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>524288</v>
+      </c>
+      <c r="B20" s="1">
+        <v>665513</v>
+      </c>
+      <c r="C20" s="1">
+        <v>928441</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>751.30012486608075</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>538.53718222267219</v>
+      </c>
+      <c r="I20">
+        <v>665513</v>
+      </c>
+      <c r="J20">
+        <v>928441</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1048576</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1332094</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1867508</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>750.69777358054307</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>535.47294041042926</v>
+      </c>
+      <c r="I21">
+        <v>1332094</v>
+      </c>
+      <c r="J21">
+        <v>1867508</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2097152</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2669499</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3741557</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>749.20425143444515</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>534.53682517732591</v>
+      </c>
+      <c r="I22">
+        <v>2669499</v>
+      </c>
+      <c r="J22">
+        <v>3741557</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>